<commit_message>
SEB XGBoost Local Results for F1 testing
</commit_message>
<xml_diff>
--- a/data/results/seb/SEB Local XGBoost Testing Results.xlsx
+++ b/data/results/seb/SEB Local XGBoost Testing Results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/results/seb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF94CB1-91C4-7641-8FA8-835126489B3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CA75C3-DD94-7F4B-BE19-6FE3CEF4ADFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="1260" windowWidth="30940" windowHeight="26220" xr2:uid="{98773DA3-37B5-D741-8ED4-95FED174B96A}"/>
+    <workbookView xWindow="39800" yWindow="4260" windowWidth="35240" windowHeight="26220" xr2:uid="{98773DA3-37B5-D741-8ED4-95FED174B96A}"/>
   </bookViews>
   <sheets>
     <sheet name="SEB TF Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Test #</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Overfitting incorrect</t>
   </si>
   <si>
-    <t xml:space="preserve">Improved precision and accuracy </t>
-  </si>
-  <si>
     <t>max_depth</t>
   </si>
   <si>
@@ -93,24 +90,15 @@
     <t>reg:squarederror</t>
   </si>
   <si>
-    <t>Initial testing and debugging</t>
-  </si>
-  <si>
     <t>First clean test</t>
   </si>
   <si>
-    <t>Overfitting incorrect but imporoved</t>
-  </si>
-  <si>
     <t>Try chaning objective to binary:logistic</t>
   </si>
   <si>
     <t>binary:logistic</t>
   </si>
   <si>
-    <t>Non converging. Only incorrect predicted.</t>
-  </si>
-  <si>
     <t>Increase epochs significantly</t>
   </si>
   <si>
@@ -126,18 +114,12 @@
     <t>Reduce epocs to see if we are overtraining.</t>
   </si>
   <si>
-    <t>Slightly Improved accuracy</t>
-  </si>
-  <si>
     <t>Adjuist Gamma to reduce overfitting</t>
   </si>
   <si>
     <t>Increase Max Depth</t>
   </si>
   <si>
-    <t>Slight loss of accuracy</t>
-  </si>
-  <si>
     <t>Increase iterations to handle depth</t>
   </si>
   <si>
@@ -150,13 +132,43 @@
     <t>Adust sub sample for more conservative model</t>
   </si>
   <si>
-    <t>Reduced accuracy</t>
-  </si>
-  <si>
     <t>Adust sub sample for more agressive model</t>
   </si>
   <si>
-    <t>Improvement</t>
+    <t>F1 Weighted</t>
+  </si>
+  <si>
+    <t>Fbeta(0.1)</t>
+  </si>
+  <si>
+    <t>Improved precision and accuracy  But same result as lower max depth</t>
+  </si>
+  <si>
+    <t>Worse with lowe subsample.</t>
+  </si>
+  <si>
+    <t>Raise Subsample</t>
+  </si>
+  <si>
+    <t>Reduced F1</t>
+  </si>
+  <si>
+    <t>Improved F1 value with same accuracy as earlier model</t>
+  </si>
+  <si>
+    <t>Seriously overfitting incorrect</t>
+  </si>
+  <si>
+    <t>More balanced but still overfitting incorrect</t>
+  </si>
+  <si>
+    <t>Improved accuracy</t>
+  </si>
+  <si>
+    <t>Silghty reduced accuracy</t>
+  </si>
+  <si>
+    <t>Unchanged</t>
   </si>
 </sst>
 </file>
@@ -166,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +187,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -203,12 +223,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -281,21 +301,6 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
       <right style="dotted">
         <color indexed="64"/>
       </right>
@@ -315,19 +320,6 @@
         <color indexed="64"/>
       </right>
       <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
@@ -398,10 +390,38 @@
       <right style="dotted">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -414,11 +434,13 @@
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -433,6 +455,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="dotted">
         <color indexed="64"/>
@@ -440,9 +501,7 @@
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -452,12 +511,19 @@
       <right style="dotted">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="dotted">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -467,6 +533,35 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="dotted">
         <color indexed="64"/>
       </top>
@@ -480,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -504,56 +599,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,28 +984,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085A1C6D-5342-E248-9087-57011A5BC40D}">
-  <dimension ref="A1:Q1048568"/>
+  <dimension ref="A1:S1048569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomLeft" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="30.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="34.1640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="34.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -898,25 +1015,25 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>3</v>
@@ -939,43 +1056,49 @@
       <c r="P1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="26">
+      <c r="B2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="11">
         <v>0.01</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="11">
         <v>4</v>
       </c>
-      <c r="E2" s="26">
-        <v>6</v>
-      </c>
-      <c r="F2" s="26">
+      <c r="E2" s="11">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="11">
         <v>0.8</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="22">
         <v>1000</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>19</v>
+      <c r="I2" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J2" s="13">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K2" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L2" s="13">
         <v>12</v>
@@ -983,25 +1106,32 @@
       <c r="M2" s="13">
         <v>5</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="15">
         <v>0.29399999999999998</v>
       </c>
-      <c r="O2" s="14">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="P2" s="14">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>10</v>
+      <c r="O2" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="P2" s="30">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q2" s="53">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="R2" s="48">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="24">
+    <row r="3" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>21</v>
+      <c r="B3" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="11">
         <v>0.01</v>
@@ -1018,43 +1148,50 @@
       <c r="G3" s="11">
         <v>0.8</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="17">
         <v>1000</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="13">
         <v>19</v>
       </c>
-      <c r="J3" s="16">
+      <c r="K3" s="13">
+        <v>6</v>
+      </c>
+      <c r="L3" s="13">
+        <v>12</v>
+      </c>
+      <c r="M3" s="13">
+        <v>6</v>
+      </c>
+      <c r="N3" s="15">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="O3" s="15">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="P3" s="30">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="Q3" s="54">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="R3" s="48">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="16">
-        <v>3</v>
-      </c>
-      <c r="L3" s="16">
-        <v>12</v>
-      </c>
-      <c r="M3" s="16">
-        <v>5</v>
-      </c>
-      <c r="N3" s="18">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="O3" s="18">
-        <v>0.625</v>
-      </c>
-      <c r="P3" s="18">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="24">
-        <v>3</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="11">
         <v>0.01</v>
@@ -1071,43 +1208,50 @@
       <c r="G4" s="11">
         <v>0.8</v>
       </c>
-      <c r="H4" s="20">
-        <v>1000</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="16">
-        <v>25</v>
-      </c>
-      <c r="K4" s="16">
-        <v>0</v>
-      </c>
-      <c r="L4" s="16">
-        <v>17</v>
-      </c>
-      <c r="M4" s="16">
-        <v>0</v>
-      </c>
-      <c r="N4" s="18">
-        <v>0</v>
-      </c>
-      <c r="O4" s="18">
-        <v>0</v>
-      </c>
-      <c r="P4" s="18">
+      <c r="H4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="13">
+        <v>19</v>
+      </c>
+      <c r="K4" s="13">
+        <v>6</v>
+      </c>
+      <c r="L4" s="13">
+        <v>11</v>
+      </c>
+      <c r="M4" s="13">
+        <v>6</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="30">
         <v>0.59499999999999997</v>
       </c>
-      <c r="Q4" s="19" t="s">
-        <v>25</v>
+      <c r="Q4" s="54">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="R4" s="48">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
+    <row r="5" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>26</v>
+      <c r="B5" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="11">
         <v>0.01</v>
@@ -1118,49 +1262,53 @@
       <c r="E5" s="11">
         <v>6</v>
       </c>
-      <c r="F5" s="11">
-        <v>1</v>
+      <c r="F5" s="12">
+        <v>6</v>
       </c>
       <c r="G5" s="11">
         <v>0.8</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="17">
         <v>10000</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="16">
-        <v>18</v>
-      </c>
-      <c r="K5" s="16">
-        <v>7</v>
-      </c>
-      <c r="L5" s="16">
-        <v>12</v>
-      </c>
-      <c r="M5" s="16">
-        <v>5</v>
-      </c>
-      <c r="N5" s="18">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="O5" s="18">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="P5" s="18">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="Q5" s="19" t="s">
+      <c r="I5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="13">
+        <v>25</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <v>15</v>
+      </c>
+      <c r="M5" s="13">
+        <v>2</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="O5" s="15">
+        <v>1</v>
+      </c>
+      <c r="P5" s="30">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q5" s="54">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="R5" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="S5" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="24">
-        <v>5</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>32</v>
+    <row r="6" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
+      <c r="B6" s="38" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="11">
         <v>0.01</v>
@@ -1172,48 +1320,55 @@
         <v>6</v>
       </c>
       <c r="F6" s="12">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G6" s="11">
         <v>0.8</v>
       </c>
-      <c r="H6" s="20">
-        <v>10000</v>
-      </c>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="17">
+        <v>1000</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="16">
-        <v>23</v>
-      </c>
-      <c r="K6" s="16">
-        <v>2</v>
-      </c>
-      <c r="L6" s="16">
-        <v>15</v>
-      </c>
-      <c r="M6" s="16">
-        <v>2</v>
-      </c>
-      <c r="N6" s="18">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="O6" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="P6" s="18">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>10</v>
+      <c r="J6" s="13">
+        <v>20</v>
+      </c>
+      <c r="K6" s="13">
+        <v>5</v>
+      </c>
+      <c r="L6" s="13">
+        <v>6</v>
+      </c>
+      <c r="M6" s="13">
+        <v>11</v>
+      </c>
+      <c r="N6" s="15">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="O6" s="15">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="P6" s="30">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="Q6" s="54">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="R6" s="48">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="S6" s="41" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24">
-        <v>6</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>27</v>
+    <row r="7" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="11">
         <v>0.01</v>
@@ -1230,96 +1385,110 @@
       <c r="G7" s="11">
         <v>0.8</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="14">
         <v>10000</v>
       </c>
       <c r="I7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="17">
+        <v>20</v>
+      </c>
+      <c r="K7" s="17">
+        <v>5</v>
+      </c>
+      <c r="L7" s="17">
+        <v>6</v>
+      </c>
+      <c r="M7" s="17">
+        <v>11</v>
+      </c>
+      <c r="N7" s="39">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="O7" s="39">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="P7" s="40">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="Q7" s="55">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="R7" s="49">
+        <v>0.76</v>
+      </c>
+      <c r="S7" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="11">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11">
+        <v>6</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="17">
+        <v>21</v>
+      </c>
+      <c r="K8" s="17">
+        <v>4</v>
+      </c>
+      <c r="L8" s="17">
+        <v>7</v>
+      </c>
+      <c r="M8" s="17">
+        <v>10</v>
+      </c>
+      <c r="N8" s="39">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="O8" s="39">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="P8" s="40">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="Q8" s="55">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R8" s="49">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="S8" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="19">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="J7" s="16">
-        <v>20</v>
-      </c>
-      <c r="K7" s="16">
-        <v>5</v>
-      </c>
-      <c r="L7" s="16">
-        <v>6</v>
-      </c>
-      <c r="M7" s="16">
-        <v>11</v>
-      </c>
-      <c r="N7" s="18">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="O7" s="18">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="P7" s="18">
-        <v>0.73799999999999999</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="24">
-        <v>7</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="37">
-        <v>0.01</v>
-      </c>
-      <c r="D8" s="37">
-        <v>4</v>
-      </c>
-      <c r="E8" s="37">
-        <v>6</v>
-      </c>
-      <c r="F8" s="37">
-        <v>6</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0.8</v>
-      </c>
-      <c r="H8" s="17">
-        <v>1000</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="38">
-        <v>21</v>
-      </c>
-      <c r="K8" s="38">
-        <v>4</v>
-      </c>
-      <c r="L8" s="38">
-        <v>6</v>
-      </c>
-      <c r="M8" s="38">
-        <v>11</v>
-      </c>
-      <c r="N8" s="39">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="O8" s="39">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="P8" s="39">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="Q8" s="40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="24">
-        <v>8</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>33</v>
       </c>
       <c r="C9" s="11">
         <v>0.01</v>
@@ -1336,43 +1505,50 @@
       <c r="G9" s="11">
         <v>0.8</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>1000</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="16">
+      <c r="I9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="13">
         <v>21</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="13">
         <v>4</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="13">
         <v>7</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="13">
         <v>10</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="15">
         <v>0.58799999999999997</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="15">
         <v>0.71399999999999997</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="30">
         <v>0.73799999999999999</v>
       </c>
-      <c r="Q9" s="19" t="s">
-        <v>34</v>
+      <c r="Q9" s="54">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="R9" s="48">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="24">
-        <v>9</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>35</v>
+    <row r="10" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="11">
         <v>0.01</v>
@@ -1389,49 +1565,56 @@
       <c r="G10" s="11">
         <v>0.8</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="14">
         <v>10000</v>
       </c>
-      <c r="I10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="16">
+      <c r="I10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="13">
         <v>21</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="13">
         <v>4</v>
       </c>
-      <c r="L10" s="16">
-        <v>6</v>
-      </c>
-      <c r="M10" s="16">
+      <c r="L10" s="13">
+        <v>6</v>
+      </c>
+      <c r="M10" s="13">
         <v>11</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="15">
         <v>0.64700000000000002</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="15">
         <v>0.73299999999999998</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="30">
         <v>0.76200000000000001</v>
       </c>
-      <c r="Q10" s="19" t="s">
-        <v>11</v>
+      <c r="Q10" s="54">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="R10" s="48">
+        <v>0.76</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="24">
-        <v>10</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>37</v>
+    <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="11">
         <v>0.01</v>
       </c>
       <c r="D11" s="11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11" s="12">
         <v>2</v>
@@ -1442,164 +1625,246 @@
       <c r="G11" s="11">
         <v>0.8</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>10000</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="16">
+      <c r="I11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="13">
         <v>20</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="13">
         <v>5</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="13">
+        <v>6</v>
+      </c>
+      <c r="M11" s="13">
+        <v>11</v>
+      </c>
+      <c r="N11" s="15">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="P11" s="30">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="Q11" s="54">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="R11" s="48">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="S11" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="12">
+        <v>10</v>
+      </c>
+      <c r="E12" s="33">
+        <v>2</v>
+      </c>
+      <c r="F12" s="33">
+        <v>6</v>
+      </c>
+      <c r="G12" s="33">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="34">
+        <v>10000</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="34">
+        <v>20</v>
+      </c>
+      <c r="K12" s="34">
         <v>5</v>
       </c>
-      <c r="M11" s="16">
+      <c r="L12" s="34">
+        <v>5</v>
+      </c>
+      <c r="M12" s="34">
         <v>12</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N12" s="35">
         <v>0.70599999999999996</v>
       </c>
-      <c r="O11" s="18">
+      <c r="O12" s="35">
         <v>0.70599999999999996</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P12" s="36">
         <v>0.76200000000000001</v>
       </c>
-      <c r="Q11" s="19" t="s">
-        <v>36</v>
+      <c r="Q12" s="56">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="R12" s="50">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="S12" s="37" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="24">
+    <row r="13" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="19">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="43">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="43">
+        <v>10</v>
+      </c>
+      <c r="E13" s="43">
+        <v>2</v>
+      </c>
+      <c r="F13" s="43">
+        <v>6</v>
+      </c>
+      <c r="G13" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="22">
+        <v>10000</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="44">
+        <v>18</v>
+      </c>
+      <c r="K13" s="44">
+        <v>7</v>
+      </c>
+      <c r="L13" s="44">
+        <v>7</v>
+      </c>
+      <c r="M13" s="44">
+        <v>10</v>
+      </c>
+      <c r="N13" s="45">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="O13" s="45">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="P13" s="46">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="Q13" s="57">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="R13" s="51">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="S13" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
+        <f>A13+1</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C14" s="20">
         <v>0.01</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D14" s="20">
         <v>10</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E14" s="20">
         <v>2</v>
       </c>
-      <c r="F12" s="11">
-        <v>6</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="F14" s="20">
+        <v>6</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="H14" s="26">
         <v>10000</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="16">
-        <v>18</v>
-      </c>
-      <c r="K12" s="16">
-        <v>7</v>
-      </c>
-      <c r="L12" s="16">
-        <v>7</v>
-      </c>
-      <c r="M12" s="16">
+      <c r="I14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="27">
         <v>10</v>
       </c>
-      <c r="N12" s="18">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="O12" s="18">
-        <v>0.58799999999999997</v>
-      </c>
-      <c r="P12" s="18">
-        <v>0.66700000000000004</v>
-      </c>
-      <c r="Q12" s="19" t="s">
+      <c r="K14" s="27">
+        <v>5</v>
+      </c>
+      <c r="L14" s="27">
+        <v>6</v>
+      </c>
+      <c r="M14" s="27">
+        <v>11</v>
+      </c>
+      <c r="N14" s="28">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="O14" s="28">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="P14" s="31">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="Q14" s="58">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="R14" s="52">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="S14" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
-        <v>12</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="25">
-        <v>0.01</v>
-      </c>
-      <c r="D13" s="25">
-        <v>10</v>
-      </c>
-      <c r="E13" s="25">
-        <v>2</v>
-      </c>
-      <c r="F13" s="25">
-        <v>6</v>
-      </c>
-      <c r="G13" s="31">
-        <v>0.9</v>
-      </c>
-      <c r="H13" s="32">
-        <v>10000</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="33">
-        <v>20</v>
-      </c>
-      <c r="K13" s="33">
-        <v>5</v>
-      </c>
-      <c r="L13" s="33">
-        <v>6</v>
-      </c>
-      <c r="M13" s="33">
-        <v>11</v>
-      </c>
-      <c r="N13" s="34">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="O13" s="34">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="P13" s="34">
-        <v>0.73799999999999999</v>
-      </c>
-      <c r="Q13" s="35" t="s">
-        <v>41</v>
-      </c>
+    <row r="17" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="2"/>
     </row>
-    <row r="16" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="2"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="1048568" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C1048568" s="26">
+    <row r="1048569" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C1048569" s="21">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>